<commit_message>
experiment 1 template specific qud
</commit_message>
<xml_diff>
--- a/notes/QUD_connectives_study.xlsx
+++ b/notes/QUD_connectives_study.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/momo/Dropbox/projects/connectives-qud/notes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFE4952A-32DE-AC44-8C19-9F0A60F660A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{006525DC-DE41-7745-A691-2991E7BBC69C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="1300" windowWidth="18660" windowHeight="19440" xr2:uid="{A459CA28-0FD4-6F4F-B37B-FA6409E291EC}"/>
+    <workbookView xWindow="-38400" yWindow="1300" windowWidth="24980" windowHeight="19440" xr2:uid="{A459CA28-0FD4-6F4F-B37B-FA6409E291EC}"/>
   </bookViews>
   <sheets>
     <sheet name="relevant QUD" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="955" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="964" uniqueCount="74">
   <si>
     <t>conjunction</t>
   </si>
@@ -244,6 +244,21 @@
   </si>
   <si>
     <t>****</t>
+  </si>
+  <si>
+    <t>&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;</t>
+  </si>
+  <si>
+    <t>filler</t>
+  </si>
+  <si>
+    <t>fillers</t>
+  </si>
+  <si>
+    <t>rt prediction</t>
+  </si>
+  <si>
+    <t>slow???</t>
   </si>
 </sst>
 </file>
@@ -309,7 +324,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -317,11 +332,79 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -331,6 +414,14 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -650,1716 +741,1778 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10C0B1CA-54BE-734F-A7AB-10C5F8C5EA2E}">
-  <dimension ref="A1:O70"/>
+  <dimension ref="A1:P70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="125" workbookViewId="0">
-      <selection activeCell="J36" sqref="J36"/>
+    <sheetView tabSelected="1" zoomScale="157" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="7" max="7" width="19.6640625" customWidth="1"/>
+    <col min="8" max="8" width="19.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="I1" t="s">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="J1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B2" t="s">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="C2" t="s">
         <v>14</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>64</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>65</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>0</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>66</v>
       </c>
       <c r="H2" t="s">
+        <v>72</v>
+      </c>
+      <c r="I2" t="s">
         <v>53</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>22</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="5">
         <v>1</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="5"/>
+      <c r="C4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="D4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="5" t="s">
-        <v>4</v>
-      </c>
       <c r="E4" s="5" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F4" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="G4" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="G4" s="5"/>
       <c r="H4" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="I4" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="J4" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="J4" s="5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B5" s="1" t="s">
+      <c r="K4" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="C5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="E5" s="1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G5" s="1"/>
       <c r="H5" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="I5" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="J5" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B6" s="1" t="s">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="C6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="E6" s="1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G6" s="1"/>
       <c r="H6" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="I6" s="1">
+        <v>57</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="J6" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B7" s="1" t="s">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="C7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="E7" s="1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G7" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G7" s="1"/>
       <c r="H7" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="I7" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="J7" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" s="5">
         <v>2</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="5"/>
+      <c r="C8" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="D8" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="5" t="s">
-        <v>4</v>
-      </c>
       <c r="E8" s="5" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F8" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G8" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G8" s="5" t="s">
-        <v>42</v>
-      </c>
       <c r="H8" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="I8" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="I8" s="5" t="s">
+      <c r="J8" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="J8" s="5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B9" s="1" t="s">
+      <c r="K8" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="C9" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="E9" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="G9" s="1"/>
       <c r="H9" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="I9" s="1">
+        <v>73</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="J9" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B10" s="1" t="s">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="C10" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="E10" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F10" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G10" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="G10" s="1"/>
       <c r="H10" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="I10" s="1">
+        <v>56</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="J10" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B11" s="1" t="s">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="C11" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="E11" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F11" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G11" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="G11" s="1"/>
       <c r="H11" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="I11" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="J11" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B12" s="2" t="s">
+    <row r="12" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C12" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="D12" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>4</v>
-      </c>
       <c r="E12" s="2" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F12" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G12" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A13" s="5">
+      <c r="H12" s="2"/>
+      <c r="I12" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="9">
         <v>3</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="10"/>
+      <c r="C13" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="D13" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="F13" s="5" t="s">
+      <c r="E13" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="G13" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="G13" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="H13" s="5" t="s">
+      <c r="H13" s="10"/>
+      <c r="I13" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="I13" s="5" t="s">
+      <c r="J13" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="J13" s="5" t="s">
+      <c r="K13" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="K13" s="5" t="s">
+      <c r="L13" s="10" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B14" s="2" t="s">
+      <c r="M13" s="12"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="C14" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="D14" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D14" s="2" t="s">
-        <v>4</v>
-      </c>
       <c r="E14" s="2" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G14" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B15" s="2" t="s">
+      <c r="H14" s="2"/>
+      <c r="I14" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="C15" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="D15" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D15" s="2" t="s">
-        <v>4</v>
-      </c>
       <c r="E15" s="2" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G15" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G15" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>55</v>
-      </c>
+      <c r="H15" s="2"/>
       <c r="I15" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="J15" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="M15" s="2" t="s">
+      <c r="N15" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="N15" s="2" t="s">
+      <c r="O15" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="O15" s="2" t="s">
+      <c r="P15" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B16" s="2" t="s">
+    <row r="16" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C16" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="D16" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D16" s="2" t="s">
-        <v>4</v>
-      </c>
       <c r="E16" s="2" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F16" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G16" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2" t="s">
-        <v>55</v>
-      </c>
+      <c r="H16" s="2"/>
       <c r="I16" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="J16" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="M16" s="2" t="s">
+      <c r="N16" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="N16" s="2" t="s">
+      <c r="O16" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="O16" s="2" t="s">
+      <c r="P16" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A17" s="5">
-        <v>4</v>
-      </c>
-      <c r="B17" s="5" t="s">
+    <row r="17" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="9">
+        <v>4</v>
+      </c>
+      <c r="B17" s="10"/>
+      <c r="C17" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="D17" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D17" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="F17" s="5" t="s">
+      <c r="E17" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="F17" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="G17" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="G17" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="H17" s="5" t="s">
+      <c r="H17" s="10"/>
+      <c r="I17" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="I17" s="5" t="s">
+      <c r="J17" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="J17" s="5" t="s">
+      <c r="K17" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="K17" s="5" t="s">
+      <c r="L17" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="M17" s="2" t="s">
+      <c r="M17" s="12"/>
+      <c r="N17" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="N17" s="2" t="s">
+      <c r="O17" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="O17" s="2" t="s">
+      <c r="P17" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B18" s="2" t="s">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="C18" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="D18" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D18" s="2" t="s">
-        <v>4</v>
-      </c>
       <c r="E18" s="2" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F18" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G18" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="M18" s="2" t="s">
+      <c r="H18" s="2"/>
+      <c r="I18" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="N18" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="N18" s="2" t="s">
+      <c r="O18" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="O18" s="2" t="s">
+      <c r="P18" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B19" s="2" t="s">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="C19" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="D19" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D19" s="2" t="s">
-        <v>4</v>
-      </c>
       <c r="E19" s="2" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F19" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G19" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2" t="s">
-        <v>55</v>
-      </c>
+      <c r="H19" s="2"/>
       <c r="I19" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="J19" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="N19" s="2" t="s">
+      <c r="O19" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="O19" s="2" t="s">
+      <c r="P19" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B20" s="3" t="s">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="C20" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="D20" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D20" s="3" t="s">
-        <v>4</v>
-      </c>
       <c r="E20" s="3" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F20" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G20" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="O20" s="2" t="s">
+      <c r="H20" s="3"/>
+      <c r="I20" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="P20" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B21" s="3" t="s">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="C21" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="D21" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D21" s="3" t="s">
-        <v>4</v>
-      </c>
       <c r="E21" s="3" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F21" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G21" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="H21" s="3"/>
       <c r="I21" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="J21" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="O21" s="2" t="s">
+      <c r="P21" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A22" s="5">
         <v>5</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B22" s="5"/>
+      <c r="C22" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="D22" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D22" s="5" t="s">
-        <v>4</v>
-      </c>
       <c r="E22" s="5" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F22" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="G22" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="G22" s="5"/>
-      <c r="H22" s="5" t="s">
+      <c r="H22" s="5"/>
+      <c r="I22" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="I22" s="5"/>
-      <c r="O22" s="2" t="s">
+      <c r="J22" s="5"/>
+      <c r="P22" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B23" s="3" t="s">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="C23" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="D23" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D23" s="3" t="s">
-        <v>4</v>
-      </c>
       <c r="E23" s="3" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F23" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G23" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G23" s="3"/>
-      <c r="H23" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B24" s="3" t="s">
+      <c r="H23" s="3"/>
+      <c r="I23" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="C24" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="D24" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D24" s="3" t="s">
-        <v>4</v>
-      </c>
       <c r="E24" s="3" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F24" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G24" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="G24" s="3"/>
-      <c r="H24" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="H24" s="3"/>
       <c r="I24" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="J24" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B25" s="3" t="s">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="C25" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="D25" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D25" s="3" t="s">
-        <v>4</v>
-      </c>
       <c r="E25" s="3" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F25" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G25" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="G25" s="3"/>
-      <c r="H25" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="H25" s="3"/>
+      <c r="I25" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A26" s="5">
         <v>6</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="B26" s="5"/>
+      <c r="C26" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C26" s="5" t="s">
+      <c r="D26" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D26" s="5" t="s">
-        <v>4</v>
-      </c>
       <c r="E26" s="5" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F26" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G26" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="G26" s="5"/>
-      <c r="H26" s="5" t="s">
+      <c r="H26" s="5"/>
+      <c r="I26" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="I26" s="5"/>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B27" s="3" t="s">
+      <c r="J26" s="5"/>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="C27" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="D27" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D27" s="3" t="s">
-        <v>4</v>
-      </c>
       <c r="E27" s="3" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F27" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G27" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G27" s="3"/>
-      <c r="H27" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="H27" s="3"/>
       <c r="I27" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="J27" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B28" s="4" t="s">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="C28" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C28" s="4" t="s">
+      <c r="D28" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D28" s="4" t="s">
-        <v>4</v>
-      </c>
       <c r="E28" s="4" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F28" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G28" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="G28" s="4"/>
-      <c r="H28" s="4" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B29" s="4" t="s">
+      <c r="H28" s="4"/>
+      <c r="I28" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="C29" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C29" s="4" t="s">
+      <c r="D29" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D29" s="4" t="s">
-        <v>4</v>
-      </c>
       <c r="E29" s="4" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F29" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G29" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="G29" s="4"/>
-      <c r="H29" s="4" t="s">
-        <v>55</v>
-      </c>
+      <c r="H29" s="4"/>
       <c r="I29" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="J29" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B30" s="4" t="s">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="C30" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C30" s="4" t="s">
+      <c r="D30" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D30" s="4" t="s">
-        <v>4</v>
-      </c>
       <c r="E30" s="4" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F30" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G30" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="G30" s="4"/>
-      <c r="H30" s="4" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="H30" s="4"/>
+      <c r="I30" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A31" s="5">
         <v>7</v>
       </c>
-      <c r="B31" s="5" t="s">
+      <c r="B31" s="5"/>
+      <c r="C31" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C31" s="5" t="s">
+      <c r="D31" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D31" s="5" t="s">
-        <v>4</v>
-      </c>
       <c r="E31" s="5" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F31" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="G31" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="G31" s="5"/>
-      <c r="H31" s="5" t="s">
+      <c r="H31" s="5"/>
+      <c r="I31" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="I31" s="5"/>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B32" s="4" t="s">
+      <c r="J31" s="5"/>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="C32" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C32" s="4" t="s">
+      <c r="D32" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D32" s="4" t="s">
-        <v>4</v>
-      </c>
       <c r="E32" s="4" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F32" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G32" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="G32" s="4"/>
-      <c r="H32" s="4" t="s">
-        <v>55</v>
-      </c>
+      <c r="H32" s="4"/>
       <c r="I32" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="J32" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B33" s="4" t="s">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C33" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C33" s="4" t="s">
+      <c r="D33" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D33" s="4" t="s">
-        <v>4</v>
-      </c>
       <c r="E33" s="4" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F33" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G33" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="G33" s="4"/>
-      <c r="H33" s="4" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B34" s="4" t="s">
+      <c r="H33" s="4"/>
+      <c r="I33" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C34" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C34" s="4" t="s">
+      <c r="D34" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D34" s="4" t="s">
-        <v>4</v>
-      </c>
       <c r="E34" s="4" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F34" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G34" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="G34" s="4"/>
-      <c r="H34" s="4" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H34" s="4"/>
+      <c r="I34" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" s="5">
         <v>8</v>
       </c>
-      <c r="B35" s="5" t="s">
+      <c r="B35" s="5"/>
+      <c r="C35" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C35" s="5" t="s">
+      <c r="D35" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D35" s="5" t="s">
-        <v>4</v>
-      </c>
       <c r="E35" s="5" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F35" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G35" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="G35" s="5"/>
-      <c r="H35" s="5" t="s">
+      <c r="H35" s="5"/>
+      <c r="I35" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="I35" s="5" t="s">
+      <c r="J35" s="5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="7"/>
-      <c r="B38" s="1" t="s">
+      <c r="B38" s="7"/>
+      <c r="C38" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="C38" s="1" t="s">
+      <c r="D38" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="D38" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F38" s="1" t="s">
+      <c r="E38" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="F38" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="G38" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="G38" s="1"/>
-      <c r="H38" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="I38" s="7"/>
-      <c r="J38" s="7"/>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A39" s="5">
+      <c r="H38" s="14"/>
+      <c r="I38" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="K38" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="L38" s="16" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="9">
         <v>9</v>
       </c>
-      <c r="B39" s="5" t="s">
+      <c r="B39" s="10"/>
+      <c r="C39" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C39" s="5" t="s">
+      <c r="D39" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D39" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E39" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="F39" s="5" t="s">
+      <c r="E39" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="F39" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="G39" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="G39" s="5" t="s">
+      <c r="H39" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="H39" s="5" t="s">
+      <c r="I39" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="I39" s="5" t="s">
+      <c r="J39" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="J39" s="5" t="s">
+      <c r="K39" s="11" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40" s="7"/>
-      <c r="B40" s="1" t="s">
+      <c r="B40" s="7"/>
+      <c r="C40" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="D40" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D40" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="E40" s="1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F40" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G40" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G40" s="1"/>
-      <c r="H40" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="I40" s="7"/>
+      <c r="H40" s="1"/>
+      <c r="I40" s="1" t="s">
+        <v>55</v>
+      </c>
       <c r="J40" s="7"/>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K40" s="7"/>
+    </row>
+    <row r="41" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" s="7"/>
-      <c r="B41" s="1" t="s">
+      <c r="B41" s="7"/>
+      <c r="C41" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C41" s="1" t="s">
+      <c r="D41" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D41" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="E41" s="1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F41" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G41" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="G41" s="1"/>
-      <c r="H41" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="I41" s="7"/>
+      <c r="H41" s="1"/>
+      <c r="I41" s="1" t="s">
+        <v>55</v>
+      </c>
       <c r="J41" s="7"/>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K41" s="7"/>
+    </row>
+    <row r="42" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42" s="7"/>
-      <c r="B42" s="1" t="s">
+      <c r="B42" s="7"/>
+      <c r="C42" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="C42" s="1" t="s">
+      <c r="D42" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="D42" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F42" s="1" t="s">
+      <c r="E42" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="F42" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="G42" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="G42" s="1"/>
-      <c r="H42" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="I42" s="7"/>
-      <c r="J42" s="7"/>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A43" s="5">
+      <c r="H42" s="14"/>
+      <c r="I42" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="K42" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="L42" s="16" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="9">
         <v>10</v>
       </c>
-      <c r="B43" s="5" t="s">
+      <c r="B43" s="10"/>
+      <c r="C43" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C43" s="5" t="s">
+      <c r="D43" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D43" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E43" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="F43" s="5" t="s">
+      <c r="E43" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="F43" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="G43" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="G43" s="5" t="s">
+      <c r="H43" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="H43" s="5" t="s">
+      <c r="I43" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="I43" s="5" t="s">
+      <c r="J43" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="J43" s="5" t="s">
+      <c r="K43" s="11" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A44" s="7"/>
-      <c r="B44" s="1" t="s">
+      <c r="B44" s="7"/>
+      <c r="C44" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C44" s="1" t="s">
+      <c r="D44" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D44" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="E44" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F44" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G44" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="G44" s="1"/>
-      <c r="H44" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="I44" s="7"/>
+      <c r="H44" s="1"/>
+      <c r="I44" s="1" t="s">
+        <v>55</v>
+      </c>
       <c r="J44" s="7"/>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K44" s="7"/>
+    </row>
+    <row r="45" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A45" s="7"/>
-      <c r="B45" s="1" t="s">
+      <c r="B45" s="7"/>
+      <c r="C45" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C45" s="1" t="s">
+      <c r="D45" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D45" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="E45" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F45" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G45" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="G45" s="1"/>
-      <c r="H45" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="I45" s="7"/>
+      <c r="H45" s="1"/>
+      <c r="I45" s="1" t="s">
+        <v>55</v>
+      </c>
       <c r="J45" s="7"/>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A46" s="5">
+      <c r="K45" s="7"/>
+    </row>
+    <row r="46" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="9">
         <v>11</v>
       </c>
-      <c r="B46" s="5" t="s">
+      <c r="B46" s="10"/>
+      <c r="C46" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C46" s="5" t="s">
+      <c r="D46" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D46" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E46" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="F46" s="5" t="s">
+      <c r="E46" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="F46" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="G46" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="G46" s="5" t="s">
+      <c r="H46" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="H46" s="5" t="s">
+      <c r="I46" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="I46" s="5" t="s">
+      <c r="J46" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="J46" s="7"/>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K46" s="7"/>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A47" s="7"/>
-      <c r="B47" s="2" t="s">
+      <c r="B47" s="7"/>
+      <c r="C47" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C47" s="2" t="s">
+      <c r="D47" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D47" s="2" t="s">
-        <v>4</v>
-      </c>
       <c r="E47" s="2" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F47" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G47" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="G47" s="2"/>
-      <c r="H47" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="I47" s="7"/>
+      <c r="H47" s="2"/>
+      <c r="I47" s="2" t="s">
+        <v>55</v>
+      </c>
       <c r="J47" s="7"/>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K47" s="7"/>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A48" s="7"/>
-      <c r="B48" s="2" t="s">
+      <c r="B48" s="7"/>
+      <c r="C48" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C48" s="2" t="s">
+      <c r="D48" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D48" s="2" t="s">
-        <v>4</v>
-      </c>
       <c r="E48" s="2" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F48" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G48" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="G48" s="2"/>
-      <c r="H48" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="I48" s="7"/>
+      <c r="H48" s="2"/>
+      <c r="I48" s="2" t="s">
+        <v>55</v>
+      </c>
       <c r="J48" s="7"/>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K48" s="7"/>
+    </row>
+    <row r="49" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A49" s="7"/>
-      <c r="B49" s="2" t="s">
+      <c r="B49" s="7"/>
+      <c r="C49" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C49" s="2" t="s">
+      <c r="D49" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D49" s="2" t="s">
-        <v>4</v>
-      </c>
       <c r="E49" s="2" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F49" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G49" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="G49" s="2"/>
-      <c r="H49" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="I49" s="7"/>
+      <c r="H49" s="2"/>
+      <c r="I49" s="2" t="s">
+        <v>55</v>
+      </c>
       <c r="J49" s="7"/>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A50" s="5">
+      <c r="K49" s="7"/>
+    </row>
+    <row r="50" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="9">
         <v>12</v>
       </c>
-      <c r="B50" s="5" t="s">
+      <c r="B50" s="10"/>
+      <c r="C50" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C50" s="5" t="s">
+      <c r="D50" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D50" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E50" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="F50" s="5" t="s">
+      <c r="E50" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="F50" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="G50" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="G50" s="5" t="s">
+      <c r="H50" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="H50" s="5" t="s">
+      <c r="I50" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="I50" s="5" t="s">
+      <c r="J50" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="J50" s="7"/>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K50" s="7"/>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A51" s="7"/>
-      <c r="B51" s="2" t="s">
+      <c r="B51" s="7"/>
+      <c r="C51" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C51" s="2" t="s">
+      <c r="D51" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D51" s="2" t="s">
-        <v>4</v>
-      </c>
       <c r="E51" s="2" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F51" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G51" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="G51" s="2"/>
-      <c r="H51" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="I51" s="7"/>
+      <c r="H51" s="2"/>
+      <c r="I51" s="2" t="s">
+        <v>55</v>
+      </c>
       <c r="J51" s="7"/>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K51" s="7"/>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A52" s="7"/>
-      <c r="B52" s="2" t="s">
+      <c r="B52" s="7"/>
+      <c r="C52" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C52" s="2" t="s">
+      <c r="D52" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D52" s="2" t="s">
-        <v>4</v>
-      </c>
       <c r="E52" s="2" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F52" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G52" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G52" s="2"/>
-      <c r="H52" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="I52" s="7"/>
+      <c r="H52" s="2"/>
+      <c r="I52" s="2" t="s">
+        <v>55</v>
+      </c>
       <c r="J52" s="7"/>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K52" s="7"/>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A53" s="7"/>
-      <c r="B53" s="2" t="s">
+      <c r="B53" s="7"/>
+      <c r="C53" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C53" s="2" t="s">
+      <c r="D53" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D53" s="2" t="s">
-        <v>4</v>
-      </c>
       <c r="E53" s="2" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F53" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G53" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="G53" s="2"/>
-      <c r="H53" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="I53" s="7"/>
+      <c r="H53" s="2"/>
+      <c r="I53" s="2" t="s">
+        <v>55</v>
+      </c>
       <c r="J53" s="7"/>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K53" s="7"/>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A54" s="7"/>
-      <c r="B54" s="3" t="s">
+      <c r="B54" s="7"/>
+      <c r="C54" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C54" s="3" t="s">
+      <c r="D54" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D54" s="3" t="s">
-        <v>4</v>
-      </c>
       <c r="E54" s="3" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F54" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G54" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="G54" s="3"/>
-      <c r="H54" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="I54" s="7"/>
+      <c r="H54" s="3"/>
+      <c r="I54" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="J54" s="7"/>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K54" s="7"/>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A55" s="7"/>
-      <c r="B55" s="3" t="s">
+      <c r="B55" s="7"/>
+      <c r="C55" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C55" s="3" t="s">
+      <c r="D55" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D55" s="3" t="s">
-        <v>4</v>
-      </c>
       <c r="E55" s="3" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F55" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G55" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="G55" s="3"/>
-      <c r="H55" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="I55" s="7"/>
+      <c r="H55" s="3"/>
+      <c r="I55" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="J55" s="7"/>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K55" s="7"/>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A56" s="5">
         <v>13</v>
       </c>
-      <c r="B56" s="5" t="s">
+      <c r="B56" s="5"/>
+      <c r="C56" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C56" s="5" t="s">
+      <c r="D56" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D56" s="5" t="s">
-        <v>4</v>
-      </c>
       <c r="E56" s="5" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F56" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="G56" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="G56" s="5" t="s">
+      <c r="H56" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="H56" s="5" t="s">
+      <c r="I56" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="I56" s="5" t="s">
+      <c r="J56" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="J56" s="7"/>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K56" s="7"/>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A57" s="7"/>
-      <c r="B57" s="3" t="s">
+      <c r="B57" s="7"/>
+      <c r="C57" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C57" s="3" t="s">
+      <c r="D57" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D57" s="3" t="s">
-        <v>4</v>
-      </c>
       <c r="E57" s="3" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F57" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G57" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="G57" s="3"/>
-      <c r="H57" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="I57" s="7"/>
+      <c r="H57" s="3"/>
+      <c r="I57" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="J57" s="7"/>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K57" s="7"/>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A58" s="7"/>
-      <c r="B58" s="3" t="s">
+      <c r="B58" s="7"/>
+      <c r="C58" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C58" s="3" t="s">
+      <c r="D58" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D58" s="3" t="s">
-        <v>4</v>
-      </c>
       <c r="E58" s="3" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F58" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G58" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="G58" s="3"/>
-      <c r="H58" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="I58" s="7"/>
+      <c r="H58" s="3"/>
+      <c r="I58" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="J58" s="7"/>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K58" s="7"/>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A59" s="7"/>
-      <c r="B59" s="3" t="s">
+      <c r="B59" s="7"/>
+      <c r="C59" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C59" s="3" t="s">
+      <c r="D59" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D59" s="3" t="s">
-        <v>4</v>
-      </c>
       <c r="E59" s="3" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F59" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G59" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="G59" s="3"/>
-      <c r="H59" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="I59" s="7"/>
+      <c r="H59" s="3"/>
+      <c r="I59" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="J59" s="7"/>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K59" s="7"/>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A60" s="5">
         <v>14</v>
       </c>
-      <c r="B60" s="5" t="s">
+      <c r="B60" s="5"/>
+      <c r="C60" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C60" s="5" t="s">
+      <c r="D60" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D60" s="5" t="s">
-        <v>4</v>
-      </c>
       <c r="E60" s="5" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F60" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G60" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="G60" s="5" t="s">
+      <c r="H60" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="H60" s="5" t="s">
+      <c r="I60" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="I60" s="5" t="s">
+      <c r="J60" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="J60" s="7"/>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K60" s="7"/>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A61" s="7"/>
-      <c r="B61" s="3" t="s">
+      <c r="B61" s="7"/>
+      <c r="C61" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C61" s="3" t="s">
+      <c r="D61" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D61" s="3" t="s">
-        <v>4</v>
-      </c>
       <c r="E61" s="3" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F61" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G61" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="G61" s="3"/>
-      <c r="H61" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="I61" s="7"/>
+      <c r="H61" s="3"/>
+      <c r="I61" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="J61" s="7"/>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K61" s="7"/>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A62" s="7"/>
-      <c r="B62" s="4" t="s">
+      <c r="B62" s="7"/>
+      <c r="C62" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C62" s="4" t="s">
+      <c r="D62" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D62" s="4" t="s">
-        <v>4</v>
-      </c>
       <c r="E62" s="4" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F62" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G62" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="G62" s="4"/>
-      <c r="H62" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="I62" s="7"/>
+      <c r="H62" s="4"/>
+      <c r="I62" s="4" t="s">
+        <v>55</v>
+      </c>
       <c r="J62" s="7"/>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K62" s="7"/>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A63" s="7"/>
-      <c r="B63" s="4" t="s">
+      <c r="B63" s="7"/>
+      <c r="C63" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C63" s="4" t="s">
+      <c r="D63" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D63" s="4" t="s">
-        <v>4</v>
-      </c>
       <c r="E63" s="4" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F63" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G63" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="G63" s="4"/>
-      <c r="H63" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="I63" s="7"/>
+      <c r="H63" s="4"/>
+      <c r="I63" s="4" t="s">
+        <v>55</v>
+      </c>
       <c r="J63" s="7"/>
-    </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K63" s="7"/>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A64" s="5">
         <v>15</v>
       </c>
-      <c r="B64" s="5" t="s">
+      <c r="B64" s="5"/>
+      <c r="C64" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C64" s="5" t="s">
+      <c r="D64" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D64" s="5" t="s">
-        <v>4</v>
-      </c>
       <c r="E64" s="5" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F64" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="G64" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="G64" s="5" t="s">
+      <c r="H64" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="H64" s="5" t="s">
+      <c r="I64" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="I64" s="5" t="s">
+      <c r="J64" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="J64" s="5" t="s">
+      <c r="K64" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="K64" s="5"/>
-    </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="L64" s="5"/>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A65" s="7"/>
-      <c r="B65" s="4" t="s">
+      <c r="B65" s="7"/>
+      <c r="C65" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C65" s="4" t="s">
+      <c r="D65" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D65" s="4" t="s">
-        <v>4</v>
-      </c>
       <c r="E65" s="4" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F65" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G65" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="G65" s="4"/>
-      <c r="H65" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="I65" s="7"/>
+      <c r="H65" s="4"/>
+      <c r="I65" s="4" t="s">
+        <v>55</v>
+      </c>
       <c r="J65" s="7"/>
-    </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K65" s="7"/>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A66" s="7"/>
-      <c r="B66" s="4" t="s">
+      <c r="B66" s="7"/>
+      <c r="C66" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C66" s="4" t="s">
+      <c r="D66" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D66" s="4" t="s">
-        <v>4</v>
-      </c>
       <c r="E66" s="4" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F66" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G66" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="G66" s="4"/>
-      <c r="H66" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="I66" s="7"/>
+      <c r="H66" s="4"/>
+      <c r="I66" s="4" t="s">
+        <v>55</v>
+      </c>
       <c r="J66" s="7"/>
-    </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K66" s="7"/>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A67" s="7"/>
-      <c r="B67" s="4" t="s">
+      <c r="B67" s="7"/>
+      <c r="C67" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C67" s="4" t="s">
+      <c r="D67" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D67" s="4" t="s">
-        <v>4</v>
-      </c>
       <c r="E67" s="4" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F67" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G67" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="G67" s="4"/>
-      <c r="H67" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="I67" s="7"/>
+      <c r="H67" s="4"/>
+      <c r="I67" s="4" t="s">
+        <v>55</v>
+      </c>
       <c r="J67" s="7"/>
-    </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K67" s="7"/>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A68" s="5">
         <v>16</v>
       </c>
-      <c r="B68" s="5" t="s">
+      <c r="B68" s="5"/>
+      <c r="C68" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C68" s="5" t="s">
+      <c r="D68" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D68" s="5" t="s">
-        <v>4</v>
-      </c>
       <c r="E68" s="5" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F68" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G68" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="G68" s="5" t="s">
+      <c r="H68" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="H68" s="5" t="s">
+      <c r="I68" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="I68" s="5" t="s">
+      <c r="J68" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="J68" s="7"/>
-    </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K68" s="7"/>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A69" s="7"/>
-      <c r="B69" s="4" t="s">
+      <c r="B69" s="7"/>
+      <c r="C69" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C69" s="4" t="s">
+      <c r="D69" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D69" s="4" t="s">
-        <v>4</v>
-      </c>
       <c r="E69" s="4" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F69" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G69" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="G69" s="4"/>
-      <c r="H69" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="I69" s="7"/>
+      <c r="H69" s="4"/>
+      <c r="I69" s="4" t="s">
+        <v>55</v>
+      </c>
       <c r="J69" s="7"/>
-    </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K69" s="7"/>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A70" s="7"/>
+      <c r="B70" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>